<commit_message>
Added pressure increase over sequential solutions to improve chance of getting a premix solution
</commit_message>
<xml_diff>
--- a/src/Burke_input_files/Burke_data.xlsx
+++ b/src/Burke_input_files/Burke_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="2080" windowWidth="37520" windowHeight="18400" activeTab="1"/>
+    <workbookView xWindow="-620" yWindow="2260" windowWidth="37520" windowHeight="18400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="118">
   <si>
     <t>phi</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>Preliminary Calc</t>
+  </si>
+  <si>
+    <t>psteps</t>
+  </si>
+  <si>
+    <t>pstart</t>
   </si>
 </sst>
 </file>
@@ -441,7 +447,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,8 +459,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -462,379 +470,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>su</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$L$3:$L$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
-                <c:pt idx="1">
-                  <c:v>55.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>58.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>23.1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>105.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>40.1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>59.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42.3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>27.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>97.7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44.3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>31.4</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>22.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>16.3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>139.3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>114.6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>95.3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>66.2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>61.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$AE$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Preliminary Calc</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$AE$3:$AE$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
-                <c:pt idx="1">
-                  <c:v>59.26400024</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39.56460048</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.47478476</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.537410739</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61.41650198</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>63.26445078</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>46.31954902</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28.66687095</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.3382031</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.245813452</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>106.1965113</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>73.35224734000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48.21404384</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>60.73717421</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>46.88075134</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>31.2779701</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20.29328704</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>12.71023919</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100.8946819</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>73.16912962</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>50.45847385</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>35.165222</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24.78989127</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>17.95615264</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>140.8768137</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>118.1077879</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>96.18610864</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>94.14821818</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>69.95420269</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>85.56884426</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>62.12325785</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2087591256"/>
-        <c:axId val="2115198248"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2087591256"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115198248"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2115198248"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087591256"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1122,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG48"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1133,29 +791,31 @@
     <col min="17" max="17" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:35">
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -1249,8 +909,14 @@
       <c r="AF2" t="s">
         <v>72</v>
       </c>
+      <c r="AG2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:35">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1346,11 +1012,18 @@
       <c r="AF4" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AG4" s="3">
+        <f>E4</f>
+        <v>1</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:35">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -1446,11 +1119,18 @@
       <c r="AF5" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AG5" s="3">
+        <f t="shared" ref="AG5:AG48" si="2">E5</f>
+        <v>5</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:35">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -1546,8 +1226,15 @@
       <c r="AF6" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG6" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:35">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -1643,8 +1330,15 @@
       <c r="AF7" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG7" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:35">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1740,8 +1434,15 @@
       <c r="AF8" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG8" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:35">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1837,8 +1538,15 @@
       <c r="AF9" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG9" s="3">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1934,8 +1642,15 @@
       <c r="AF10" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG10" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:35">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -2031,8 +1746,15 @@
       <c r="AF11" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG11" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:35">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2128,8 +1850,15 @@
       <c r="AF12" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG12" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:35">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -2225,8 +1954,15 @@
       <c r="AF13" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG13" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:35">
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -2322,11 +2058,18 @@
       <c r="AF14" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AG14" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:35">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -2422,8 +2165,15 @@
       <c r="AF15" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG15" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:35">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -2519,8 +2269,15 @@
       <c r="AF16" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG16" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="2:32">
+    <row r="17" spans="2:34">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -2616,8 +2373,15 @@
       <c r="AF17" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG17" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="2:32">
+    <row r="18" spans="2:34">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -2713,8 +2477,15 @@
       <c r="AF18" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG18" s="3">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="2:32">
+    <row r="19" spans="2:34">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -2810,8 +2581,15 @@
       <c r="AF19" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG19" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="2:32">
+    <row r="20" spans="2:34">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -2907,8 +2685,15 @@
       <c r="AF20" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG20" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="2:32">
+    <row r="21" spans="2:34">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -3004,8 +2789,15 @@
       <c r="AF21" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG21" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="2:32">
+    <row r="22" spans="2:34">
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -3101,8 +2893,15 @@
       <c r="AF22" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG22" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="2:32">
+    <row r="23" spans="2:34">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -3198,8 +2997,15 @@
       <c r="AF23" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG23" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH23" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="2:32">
+    <row r="24" spans="2:34">
       <c r="B24" t="s">
         <v>35</v>
       </c>
@@ -3295,8 +3101,15 @@
       <c r="AF24" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG24" s="3">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AH24" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="2:32">
+    <row r="25" spans="2:34">
       <c r="B25" t="s">
         <v>36</v>
       </c>
@@ -3392,8 +3205,15 @@
       <c r="AF25" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG25" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH25" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="2:32">
+    <row r="26" spans="2:34">
       <c r="B26" t="s">
         <v>37</v>
       </c>
@@ -3489,8 +3309,15 @@
       <c r="AF26" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG26" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH26" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="2:32">
+    <row r="27" spans="2:34">
       <c r="B27" t="s">
         <v>38</v>
       </c>
@@ -3586,8 +3413,15 @@
       <c r="AF27" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG27" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH27" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="2:32">
+    <row r="28" spans="2:34">
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -3683,8 +3517,15 @@
       <c r="AF28" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG28" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH28" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="2:32">
+    <row r="29" spans="2:34">
       <c r="B29" t="s">
         <v>40</v>
       </c>
@@ -3780,8 +3621,15 @@
       <c r="AF29" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG29" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH29" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="2:32">
+    <row r="30" spans="2:34">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -3877,8 +3725,15 @@
       <c r="AF30" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG30" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH30" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="2:32">
+    <row r="31" spans="2:34">
       <c r="B31" t="s">
         <v>42</v>
       </c>
@@ -3974,8 +3829,15 @@
       <c r="AF31" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG31" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH31" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="2:32">
+    <row r="32" spans="2:34">
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -4071,8 +3933,15 @@
       <c r="AF32" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG32" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH32" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="2:32">
+    <row r="33" spans="2:34">
       <c r="B33" t="s">
         <v>44</v>
       </c>
@@ -4168,8 +4037,15 @@
       <c r="AF33" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG33" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH33" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="2:32">
+    <row r="34" spans="2:34">
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -4265,8 +4141,15 @@
       <c r="AF34" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG34" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH34" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="2:32">
+    <row r="35" spans="2:34">
       <c r="B35" t="s">
         <v>46</v>
       </c>
@@ -4362,8 +4245,15 @@
       <c r="AF35" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG35" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH35" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="2:32">
+    <row r="36" spans="2:34">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -4459,8 +4349,15 @@
       <c r="AF36" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG36" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH36" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="2:32">
+    <row r="37" spans="2:34">
       <c r="B37" t="s">
         <v>48</v>
       </c>
@@ -4556,8 +4453,15 @@
       <c r="AF37" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG37" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH37" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="2:32">
+    <row r="38" spans="2:34">
       <c r="B38" t="s">
         <v>49</v>
       </c>
@@ -4653,8 +4557,15 @@
       <c r="AF38" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG38" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH38" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="2:32">
+    <row r="39" spans="2:34">
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -4750,8 +4661,15 @@
       <c r="AF39" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG39" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH39" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="2:32">
+    <row r="40" spans="2:34">
       <c r="B40" t="s">
         <v>51</v>
       </c>
@@ -4847,8 +4765,15 @@
       <c r="AF40" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG40" s="3">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AH40" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="2:32">
+    <row r="41" spans="2:34">
       <c r="B41" t="s">
         <v>52</v>
       </c>
@@ -4944,8 +4869,15 @@
       <c r="AF41" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG41" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH41" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="2:32">
+    <row r="42" spans="2:34">
       <c r="B42" t="s">
         <v>53</v>
       </c>
@@ -5041,8 +4973,15 @@
       <c r="AF42" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG42" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH42" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="2:32">
+    <row r="43" spans="2:34">
       <c r="B43" t="s">
         <v>54</v>
       </c>
@@ -5138,8 +5077,15 @@
       <c r="AF43" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG43" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AH43" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="2:32">
+    <row r="44" spans="2:34">
       <c r="B44" t="s">
         <v>55</v>
       </c>
@@ -5235,8 +5181,15 @@
       <c r="AF44" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG44" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="AH44" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="2:32">
+    <row r="45" spans="2:34">
       <c r="B45" t="s">
         <v>56</v>
       </c>
@@ -5332,8 +5285,15 @@
       <c r="AF45" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG45" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AH45" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="2:32">
+    <row r="46" spans="2:34">
       <c r="B46" t="s">
         <v>57</v>
       </c>
@@ -5429,8 +5389,15 @@
       <c r="AF46" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG46" s="3">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AH46" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="2:32">
+    <row r="47" spans="2:34">
       <c r="B47" t="s">
         <v>58</v>
       </c>
@@ -5526,8 +5493,15 @@
       <c r="AF47" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="AG47" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH47" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="2:32">
+    <row r="48" spans="2:34">
       <c r="B48" t="s">
         <v>59</v>
       </c>
@@ -5622,6 +5596,13 @@
       </c>
       <c r="AF48" s="3">
         <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AG48" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AH48" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5641,10 +5622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE35"/>
+  <dimension ref="A1:AG35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB43" sqref="AB43"/>
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5653,29 +5634,31 @@
     <col min="15" max="15" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:33">
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -5764,53 +5747,59 @@
         <v>72</v>
       </c>
       <c r="AE2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:33">
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>0.3</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>1400</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
         <v>0.1071</v>
       </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
         <v>0.17849999999999999</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <v>0.71440000000000003</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="6">
         <v>0.6</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="6">
         <v>1.5</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>55.4</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="6">
         <v>0.02</v>
       </c>
-      <c r="N4" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="O4" s="5">
+      <c r="N4" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="O4" s="6">
         <f>L4/M4*N4</f>
         <v>2.77</v>
       </c>
@@ -5860,54 +5849,61 @@
       <c r="AD4" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="3">
+        <f>E4</f>
+        <v>1</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4">
         <v>59.264000240000001</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:33">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>0.3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>1400</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>2.5</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>0.1071</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
         <v>0.17849999999999999</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <v>0.71440000000000003</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="6">
         <v>0.6</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="6">
         <v>1.5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>34</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="6">
         <f t="shared" ref="O5:O35" si="0">L5/M5*N5</f>
         <v>3.2903225806451615</v>
       </c>
@@ -5957,11 +5953,18 @@
       <c r="AD5" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="3">
+        <f t="shared" ref="AE5:AE35" si="2">E5</f>
+        <v>2.5</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5">
         <v>39.564600480000003</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:33">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6021,14 +6024,14 @@
         <v>0.7</v>
       </c>
       <c r="T6" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="U6" s="2">
         <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
       <c r="V6" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="W6" s="3">
         <v>1E-8</v>
@@ -6054,11 +6057,17 @@
       <c r="AD6" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG6">
         <v>39.474784759999999</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:33">
       <c r="A7">
         <v>3</v>
       </c>
@@ -6118,7 +6127,7 @@
         <v>0.7</v>
       </c>
       <c r="T7" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="U7" s="2">
         <f t="shared" si="1"/>
@@ -6151,54 +6160,60 @@
       <c r="AD7" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>10</v>
+      </c>
+      <c r="AG7">
         <v>5.5374107390000002</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:33">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>0.3</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>1600</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>5</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>0.1305</v>
       </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
         <v>0.2175</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <v>0.65190000000000003</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="6">
         <v>0.6</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="6">
         <v>1.5</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>58.2</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="6">
         <v>0.11799999999999999</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="6">
         <f t="shared" si="0"/>
         <v>1.9728813559322036</v>
       </c>
@@ -6248,51 +6263,58 @@
       <c r="AD8" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG8">
         <v>61.41650198</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:33">
+      <c r="B9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>0.5</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>1400</v>
       </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
         <v>0.1026</v>
       </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
         <v>0.1026</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <v>0.79479999999999995</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="6">
         <v>0.6</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="6">
         <v>1.5</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="6">
         <v>61</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="N9" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="O9" s="5">
+      <c r="N9" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="O9" s="6">
         <f t="shared" si="0"/>
         <v>3.5882352941176467</v>
       </c>
@@ -6342,51 +6364,58 @@
       <c r="AD9" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9">
         <v>63.264450779999997</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:33">
+      <c r="B10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>0.5</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>1400</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <v>2.5</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>0.1026</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
         <v>0.1026</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <v>0.79479999999999995</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="6">
         <v>0.6</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="6">
         <v>1.5</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="6">
         <v>37.9</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="6">
         <f t="shared" si="0"/>
         <v>4.3730769230769226</v>
       </c>
@@ -6436,51 +6465,58 @@
       <c r="AD10" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG10">
         <v>46.319549019999997</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:33">
+      <c r="B11" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>0.5</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>1400</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>5</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>0.1026</v>
       </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
         <v>0.1026</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="6">
         <v>0.79479999999999995</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="6">
         <v>0.6</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="6">
         <v>1.5</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="6">
         <v>23.1</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="6">
         <f t="shared" si="0"/>
         <v>2.1656249999999999</v>
       </c>
@@ -6530,11 +6566,18 @@
       <c r="AD11" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11">
         <v>28.66687095</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:33">
       <c r="B12" t="s">
         <v>90</v>
       </c>
@@ -6591,7 +6634,7 @@
         <v>0.7</v>
       </c>
       <c r="T12" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U12" s="2">
         <f t="shared" si="1"/>
@@ -6624,11 +6667,17 @@
       <c r="AD12" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG12">
         <v>16.338203100000001</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:33">
       <c r="B13" t="s">
         <v>91</v>
       </c>
@@ -6685,7 +6734,7 @@
         <v>0.7</v>
       </c>
       <c r="T13" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="U13" s="2">
         <f t="shared" si="1"/>
@@ -6718,11 +6767,17 @@
       <c r="AD13" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="3">
+        <v>5</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>20</v>
+      </c>
+      <c r="AG13">
         <v>9.2458134520000002</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:33">
       <c r="B14" t="s">
         <v>92</v>
       </c>
@@ -6779,7 +6834,7 @@
         <v>0.7</v>
       </c>
       <c r="T14" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" si="1"/>
@@ -6812,51 +6867,57 @@
       <c r="AD14" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="3">
+        <v>5</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>15</v>
+      </c>
+      <c r="AG14">
         <v>106.1965113</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:33">
+      <c r="B15" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>0.5</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>1600</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <v>5</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>0.1236</v>
       </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
         <v>0.1236</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="6">
         <v>0.75280000000000002</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="6">
         <v>0.5</v>
       </c>
-      <c r="K15" s="5">
-        <v>1</v>
-      </c>
-      <c r="L15" s="5">
+      <c r="K15" s="6">
+        <v>1</v>
+      </c>
+      <c r="L15" s="6">
         <v>64.3</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="6">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="6">
         <f t="shared" si="0"/>
         <v>2.6791666666666667</v>
       </c>
@@ -6906,51 +6967,58 @@
       <c r="AD15" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE15">
+      <c r="AE15" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG15">
         <v>73.352247340000005</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="1:33">
+      <c r="B16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>0.5</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>1600</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>10</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>0.1236</v>
       </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
         <v>0.1236</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="6">
         <v>0.75280000000000002</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="6">
         <v>0.5</v>
       </c>
-      <c r="K16" s="5">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5">
+      <c r="K16" s="6">
+        <v>1</v>
+      </c>
+      <c r="L16" s="6">
         <v>40.1</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="6">
         <v>0.12</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O16" s="5">
+      <c r="O16" s="6">
         <f t="shared" si="0"/>
         <v>1.6708333333333334</v>
       </c>
@@ -7000,51 +7068,58 @@
       <c r="AD16" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE16">
+      <c r="AE16" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG16">
         <v>48.214043840000002</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:33">
+      <c r="B17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>0.7</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>1400</v>
       </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5">
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
         <v>0.1008</v>
       </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="6">
         <v>0.82720000000000005</v>
       </c>
-      <c r="J17" s="5">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5">
+      <c r="J17" s="6">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6">
         <v>2.5</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="6">
         <v>59.7</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="N17" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="O17" s="5">
+      <c r="N17" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="O17" s="6">
         <f t="shared" si="0"/>
         <v>4.2642857142857151</v>
       </c>
@@ -7094,51 +7169,58 @@
       <c r="AD17" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE17">
+      <c r="AE17" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG17">
         <v>60.737174209999999</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="1:33">
+      <c r="B18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>0.7</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>1400</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>2.5</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>0.1008</v>
       </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="6">
         <v>0.82720000000000005</v>
       </c>
-      <c r="J18" s="5">
-        <v>1</v>
-      </c>
-      <c r="K18" s="5">
+      <c r="J18" s="6">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6">
         <v>2.5</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="6">
         <v>42.3</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="6">
         <v>2E-3</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="6">
         <f t="shared" si="0"/>
         <v>3.3839999999999995</v>
       </c>
@@ -7188,51 +7270,58 @@
       <c r="AD18" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18">
         <v>46.880751340000003</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:33">
+      <c r="B19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>0.7</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>1400</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>5</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
         <v>0.1008</v>
       </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="6">
         <v>0.82720000000000005</v>
       </c>
-      <c r="J19" s="5">
-        <v>1</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="J19" s="6">
+        <v>1</v>
+      </c>
+      <c r="K19" s="6">
         <v>2.5</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="6">
         <v>27.6</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="6">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="6">
         <v>2E-3</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="6">
         <f t="shared" si="0"/>
         <v>1.6727272727272728</v>
       </c>
@@ -7282,11 +7371,18 @@
       <c r="AD19" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19">
         <v>31.277970100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:33">
       <c r="B20" t="s">
         <v>98</v>
       </c>
@@ -7343,7 +7439,7 @@
         <v>0.7</v>
       </c>
       <c r="T20" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" si="1"/>
@@ -7376,11 +7472,18 @@
       <c r="AD20" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE20">
+      <c r="AE20" s="3">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG20">
         <v>20.293287039999999</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:33">
       <c r="B21" t="s">
         <v>99</v>
       </c>
@@ -7437,7 +7540,7 @@
         <v>0.7</v>
       </c>
       <c r="T21" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U21" s="2">
         <f t="shared" si="1"/>
@@ -7470,51 +7573,57 @@
       <c r="AD21" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE21">
+      <c r="AE21" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG21">
         <v>12.710239189999999</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
-      <c r="B22" s="5" t="s">
+    <row r="22" spans="1:33">
+      <c r="B22" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>0.7</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>1600</v>
       </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
         <v>0.12089999999999999</v>
       </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
         <v>8.6300000000000002E-2</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="6">
         <v>0.79279999999999995</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="6">
         <v>0.5</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="6">
         <v>1.5</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L22" s="6">
         <v>97.7</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="N22" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="O22" s="5">
+      <c r="N22" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="O22" s="6">
         <f t="shared" si="0"/>
         <v>3.9079999999999999</v>
       </c>
@@ -7564,51 +7673,58 @@
       <c r="AD22" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE22">
+      <c r="AE22" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG22">
         <v>100.89468189999999</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="1:33">
+      <c r="B23" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>0.7</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>1600</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="6">
         <v>5</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>0.12089999999999999</v>
       </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6">
         <v>8.6300000000000002E-2</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="6">
         <v>0.79279999999999995</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="6">
         <v>0.5</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="6">
         <v>1.5</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23" s="6">
         <v>67</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="6">
         <f t="shared" si="0"/>
         <v>3.1529411764705877</v>
       </c>
@@ -7658,11 +7774,18 @@
       <c r="AD23" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE23">
+      <c r="AE23" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG23">
         <v>73.169129620000007</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:33">
       <c r="B24" t="s">
         <v>102</v>
       </c>
@@ -7719,7 +7842,7 @@
         <v>0.7</v>
       </c>
       <c r="T24" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U24" s="2">
         <f t="shared" si="1"/>
@@ -7752,11 +7875,17 @@
       <c r="AD24" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE24">
+      <c r="AE24" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="AF24" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG24">
         <v>50.458473849999997</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:33">
       <c r="B25" t="s">
         <v>103</v>
       </c>
@@ -7813,7 +7942,7 @@
         <v>0.7</v>
       </c>
       <c r="T25" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U25" s="2">
         <f t="shared" si="1"/>
@@ -7846,11 +7975,17 @@
       <c r="AD25" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE25">
+      <c r="AE25" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="AF25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG25">
         <v>35.165222</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:33">
       <c r="B26" t="s">
         <v>104</v>
       </c>
@@ -7907,7 +8042,7 @@
         <v>0.7</v>
       </c>
       <c r="T26" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U26" s="2">
         <f t="shared" si="1"/>
@@ -7940,11 +8075,17 @@
       <c r="AD26" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE26">
+      <c r="AE26" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="AF26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG26">
         <v>24.789891269999998</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:33">
       <c r="B27" t="s">
         <v>105</v>
       </c>
@@ -8001,7 +8142,7 @@
         <v>0.7</v>
       </c>
       <c r="T27" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U27" s="2">
         <f t="shared" si="1"/>
@@ -8034,51 +8175,57 @@
       <c r="AD27" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE27">
+      <c r="AE27" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="AF27" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG27">
         <v>17.956152639999999</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="1:33">
+      <c r="B28" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="6">
         <v>0.7</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>1800</v>
       </c>
-      <c r="E28" s="5">
-        <v>1</v>
-      </c>
-      <c r="F28" s="5">
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
         <v>0.1406</v>
       </c>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5">
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6">
         <v>0.1004</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="6">
         <v>0.75900000000000001</v>
       </c>
-      <c r="J28" s="5">
-        <v>1</v>
-      </c>
-      <c r="K28" s="5">
+      <c r="J28" s="6">
+        <v>1</v>
+      </c>
+      <c r="K28" s="6">
         <v>2.5</v>
       </c>
-      <c r="L28" s="5">
+      <c r="L28" s="6">
         <v>139.30000000000001</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="N28" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="O28" s="5">
+      <c r="N28" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="O28" s="6">
         <f t="shared" si="0"/>
         <v>3.6657894736842112</v>
       </c>
@@ -8128,51 +8275,58 @@
       <c r="AD28" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE28">
+      <c r="AE28" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG28">
         <v>140.87681370000001</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="1:33">
+      <c r="B29" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="6">
         <v>0.7</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>1800</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="6">
         <v>5</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="6">
         <v>0.1406</v>
       </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
         <v>0.1004</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="6">
         <v>0.75900000000000001</v>
       </c>
-      <c r="J29" s="5">
-        <v>1</v>
-      </c>
-      <c r="K29" s="5">
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+      <c r="K29" s="6">
         <v>2.5</v>
       </c>
-      <c r="L29" s="5">
+      <c r="L29" s="6">
         <v>114.6</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29" s="6">
         <v>0.155</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N29" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="O29" s="5">
+      <c r="O29" s="6">
         <f t="shared" si="0"/>
         <v>4.4361290322580649</v>
       </c>
@@ -8222,51 +8376,58 @@
       <c r="AD29" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE29">
+      <c r="AE29" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG29">
         <v>118.10778790000001</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
-      <c r="B30" s="5" t="s">
+    <row r="30" spans="1:33">
+      <c r="B30" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="6">
         <v>0.7</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="6">
         <v>1800</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="6">
         <v>10</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="6">
         <v>0.1406</v>
       </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="5">
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
         <v>0.1004</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="6">
         <v>0.75900000000000001</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="6">
         <v>0.5</v>
       </c>
-      <c r="K30" s="5">
+      <c r="K30" s="6">
         <v>1.5</v>
       </c>
-      <c r="L30" s="5">
+      <c r="L30" s="6">
         <v>96</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30" s="6">
         <v>0.25900000000000001</v>
       </c>
-      <c r="N30" s="5">
+      <c r="N30" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O30" s="5">
+      <c r="O30" s="6">
         <f t="shared" si="0"/>
         <v>3.3359073359073355</v>
       </c>
@@ -8316,15 +8477,22 @@
       <c r="AD30" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE30">
+      <c r="AE30" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AF30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG30">
         <v>96.18610864</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:33">
       <c r="A31" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C31" s="1">
@@ -8413,15 +8581,22 @@
       <c r="AD31" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE31">
+      <c r="AE31" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG31">
         <v>94.148218180000001</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:33">
       <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C32" s="1">
@@ -8510,12 +8685,19 @@
       <c r="AD32" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE32">
+      <c r="AE32" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG32">
         <v>69.954202690000002</v>
       </c>
     </row>
-    <row r="33" spans="2:31">
-      <c r="B33" s="5" t="s">
+    <row r="33" spans="2:33">
+      <c r="B33" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C33" s="1">
@@ -8604,11 +8786,18 @@
       <c r="AD33" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE33">
+      <c r="AE33" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG33">
         <v>85.568844260000006</v>
       </c>
     </row>
-    <row r="34" spans="2:31">
+    <row r="34" spans="2:33">
       <c r="B34" t="s">
         <v>112</v>
       </c>
@@ -8665,7 +8854,7 @@
         <v>0.7</v>
       </c>
       <c r="T34" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U34" s="2">
         <f t="shared" si="1"/>
@@ -8698,11 +8887,18 @@
       <c r="AD34" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AE34">
+      <c r="AE34" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AF34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG34">
         <v>62.123257850000002</v>
       </c>
     </row>
-    <row r="35" spans="2:31">
+    <row r="35" spans="2:33">
       <c r="B35" t="s">
         <v>113</v>
       </c>
@@ -8759,7 +8955,7 @@
         <v>0.7</v>
       </c>
       <c r="T35" s="2">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U35" s="2">
         <f t="shared" si="1"/>
@@ -8791,6 +8987,13 @@
       </c>
       <c r="AD35" s="3">
         <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AE35" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AF35" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8799,7 +9002,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added charts comparing data and simulation
</commit_message>
<xml_diff>
--- a/src/Burke_input_files/Burke_data.xlsx
+++ b/src/Burke_input_files/Burke_data.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1500" windowWidth="34760" windowHeight="19720" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="1500" windowWidth="34760" windowHeight="19720" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="C&amp;F 2010" sheetId="4" r:id="rId4"/>
+    <sheet name="symposium" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="122">
   <si>
     <t>Burke C&amp;F 2010 data</t>
   </si>
@@ -385,6 +387,9 @@
   <si>
     <t>k3</t>
   </si>
+  <si>
+    <t>sim</t>
+  </si>
 </sst>
 </file>
 
@@ -462,12 +467,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -494,15 +501,1311 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>su</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$3:$B$48</c:f>
+              <c:strCache>
+                <c:ptCount val="46"/>
+                <c:pt idx="1">
+                  <c:v>Burkef1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Burkef2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Burkef3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Burkef4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Burkef5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Burkef6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Burkef7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Burkef8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Burkef9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Burkef10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Burkef11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Burkef12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Burkef13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Burkef14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Burkef15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Burkef16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Burkef17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Burkef18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Burkef19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Burkef20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Burkef21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Burkef22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Burkef23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Burkef24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Burkef25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Burkef26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Burkef27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Burkef28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Burkef29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Burkef30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Burkef31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Burkef32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Burkef33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Burkef34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Burkef35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Burkef36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Burkef37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Burkef38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Burkef39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Burkef40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Burkef41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Burkef42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Burkef43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Burkef44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Burkef45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$3:$N$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="1">
+                  <c:v>95.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>105.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>104.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>78.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>53.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>123.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>103.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>75.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>54.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39.1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>27.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>147.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>121.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>100.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>63.1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>51.4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>177.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>164.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AM$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$3:$B$48</c:f>
+              <c:strCache>
+                <c:ptCount val="46"/>
+                <c:pt idx="1">
+                  <c:v>Burkef1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Burkef2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Burkef3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Burkef4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Burkef5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Burkef6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Burkef7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Burkef8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Burkef9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Burkef10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Burkef11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Burkef12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Burkef13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Burkef14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Burkef15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Burkef16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Burkef17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Burkef18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Burkef19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Burkef20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Burkef21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Burkef22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Burkef23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Burkef24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Burkef25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Burkef26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Burkef27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Burkef28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Burkef29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Burkef30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Burkef31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Burkef32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Burkef33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Burkef34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Burkef35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Burkef36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Burkef37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Burkef38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Burkef39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Burkef40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Burkef41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Burkef42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Burkef43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Burkef44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Burkef45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AM$3:$AM$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="1">
+                  <c:v>95.93723534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.57080691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.90396669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.52367952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.55322194</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.96880099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.41738964</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.01431876</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.06451469</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86.6208807</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.73040044</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45.24507887</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.68477929</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.89041847</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.85782549</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104.7389546</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>84.3676755</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>67.17508866999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50.64993755</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41.14765223</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>33.1031681</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>123.2076346</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>104.4363992</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>87.66867651</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74.49214989</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>62.78894483</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>101.8299902</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>72.67148729</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49.56766143</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.63756146</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.38514964</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>127.4196888</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100.7064265</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>76.09382294</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>58.80019865</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>46.26029896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.02144953</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>156.4556196</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>128.6319518</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>112.0877352</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>98.26918543</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>83.35072676</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>70.85534201999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>190.5931806</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>169.4175434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2087125400"/>
+        <c:axId val="2087128376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2087125400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2087128376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2087128376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2087125400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>su</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$3:$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="1">
+                  <c:v>Burkef46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Burkef47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Burkef48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Burkef49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Burkef50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Burkef51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Burkef52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Burkef53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Burkef54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Burkef55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Burkef56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Burkef57</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Burkef58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Burkef59</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Burkef60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Burkef61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Burkef62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Burkef63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Burkef64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Burkef65</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Burkef66</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Burkef67</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Burkef68</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Burkef69</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Burkef70</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Burkef71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Burkef72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Burkef73</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Burkef74</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Burkef75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Burkef76</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Burkef77</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$L$3:$L$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="1">
+                  <c:v>55.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>97.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>139.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>114.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>95.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>66.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$AK$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$3:$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="1">
+                  <c:v>Burkef46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Burkef47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Burkef48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Burkef49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Burkef50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Burkef51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Burkef52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Burkef53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Burkef54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Burkef55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Burkef56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Burkef57</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Burkef58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Burkef59</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Burkef60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Burkef61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Burkef62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Burkef63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Burkef64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Burkef65</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Burkef66</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Burkef67</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Burkef68</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Burkef69</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Burkef70</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Burkef71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Burkef72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Burkef73</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Burkef74</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Burkef75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Burkef76</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Burkef77</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$AK$3:$AK$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="1">
+                  <c:v>60.18928842</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.68335947</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.45154434</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.746588502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63.72645036</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.27190569</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.26187945</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.100196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.06638985</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.506853864</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>111.6510688</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75.65622255</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50.12831731</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61.79824247</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47.71671067</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32.10495027</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20.93472368</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.12922018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>102.3333861</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75.0626419</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.4982414</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>37.05756274</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26.28656697</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.93368352</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>142.8229451</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>121.0271814</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>98.45672097</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>95.93723534</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>71.57080691</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>86.6208807</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60.75283528</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43.42201118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2121271544"/>
+        <c:axId val="2118106664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2121271544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118106664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118106664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121271544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8570599" cy="5825269"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8570599" cy="5825269"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -827,13 +2130,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM1000"/>
+  <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ4" sqref="AJ4:AL48"/>
+      <selection pane="bottomRight" activeCell="AM2" activeCellId="2" sqref="B2:B48 N2:N48 AM2:AM48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -860,10 +2163,11 @@
     <col min="36" max="36" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.6640625" customWidth="1"/>
+    <col min="39" max="39" width="9.83203125" customWidth="1"/>
+    <col min="40" max="40" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="13.5" customHeight="1">
+    <row r="1" spans="1:40" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,8 +2195,9 @@
       <c r="AJ1" s="14"/>
       <c r="AK1" s="14"/>
       <c r="AL1" s="14"/>
-    </row>
-    <row r="2" spans="1:39" s="12" customFormat="1" ht="13.5" customHeight="1">
+      <c r="AM1" s="24"/>
+    </row>
+    <row r="2" spans="1:40" s="12" customFormat="1" ht="13.5" customHeight="1">
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1004,11 +2309,14 @@
       <c r="AL2" s="13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM2" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="13.5" customHeight="1">
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:39" ht="13.5" customHeight="1">
+    <row r="4" spans="1:40" ht="13.5" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
@@ -1123,11 +2431,14 @@
       <c r="AL4" s="20">
         <v>2</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AM4" s="25">
+        <v>95.937235340000001</v>
+      </c>
+      <c r="AN4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="13.5" customHeight="1">
+    <row r="5" spans="1:40" ht="13.5" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1242,11 +2553,14 @@
       <c r="AL5" s="20">
         <v>2</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AM5" s="25">
+        <v>71.570806910000002</v>
+      </c>
+      <c r="AN5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="13.5" customHeight="1">
+    <row r="6" spans="1:40" ht="13.5" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1361,8 +2675,11 @@
       <c r="AL6" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM6" s="25">
+        <v>52.903966689999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="13.5" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1476,8 +2793,11 @@
       <c r="AL7" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM7" s="25">
+        <v>36.523679520000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="13.5" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1592,8 +2912,11 @@
       <c r="AL8" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM8" s="25">
+        <v>26.55322194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="13.5" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>42</v>
       </c>
@@ -1706,8 +3029,11 @@
       <c r="AL9" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM9" s="25">
+        <v>19.968800989999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="13.5" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
@@ -1821,8 +3147,11 @@
       <c r="AL10" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM10" s="25">
+        <v>70.417389639999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="13.5" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
@@ -1936,8 +3265,11 @@
       <c r="AL11" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM11" s="25">
+        <v>45.014318760000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="13.5" customHeight="1">
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
@@ -2051,8 +3383,11 @@
       <c r="AL12" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM12" s="25">
+        <v>28.064514689999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="13.5" customHeight="1">
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
@@ -2167,8 +3502,11 @@
       <c r="AL13" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM13" s="25">
+        <v>86.620880700000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="13.5" customHeight="1">
       <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
@@ -2282,11 +3620,14 @@
       <c r="AL14" s="20">
         <v>2</v>
       </c>
-      <c r="AM14" s="1" t="s">
+      <c r="AM14" s="25">
+        <v>61.730400439999997</v>
+      </c>
+      <c r="AN14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="13.5" customHeight="1">
+    <row r="15" spans="1:40" ht="13.5" customHeight="1">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -2400,8 +3741,11 @@
       <c r="AL15" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" ht="13.5" customHeight="1">
+      <c r="AM15" s="25">
+        <v>45.24507887</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="13.5" customHeight="1">
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
@@ -2515,8 +3859,11 @@
       <c r="AL16" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM16" s="25">
+        <v>32.684779290000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:39" ht="13.5" customHeight="1">
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2630,8 +3977,11 @@
       <c r="AL17" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM17" s="25">
+        <v>23.89041847</v>
+      </c>
+    </row>
+    <row r="18" spans="2:39" ht="13.5" customHeight="1">
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2745,8 +4095,11 @@
       <c r="AL18" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM18" s="25">
+        <v>17.85782549</v>
+      </c>
+    </row>
+    <row r="19" spans="2:39" ht="13.5" customHeight="1">
       <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
@@ -2861,8 +4214,11 @@
       <c r="AL19" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM19" s="25">
+        <v>104.7389546</v>
+      </c>
+    </row>
+    <row r="20" spans="2:39" ht="13.5" customHeight="1">
       <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2977,8 +4333,11 @@
       <c r="AL20" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM20" s="25">
+        <v>84.367675500000004</v>
+      </c>
+    </row>
+    <row r="21" spans="2:39" ht="13.5" customHeight="1">
       <c r="B21" s="1" t="s">
         <v>56</v>
       </c>
@@ -3093,8 +4452,11 @@
       <c r="AL21" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM21" s="25">
+        <v>67.175088669999994</v>
+      </c>
+    </row>
+    <row r="22" spans="2:39" ht="13.5" customHeight="1">
       <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3208,8 +4570,11 @@
       <c r="AL22" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM22" s="25">
+        <v>50.649937549999997</v>
+      </c>
+    </row>
+    <row r="23" spans="2:39" ht="13.5" customHeight="1">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
@@ -3323,8 +4688,11 @@
       <c r="AL23" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM23" s="25">
+        <v>41.147652229999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:39" ht="13.5" customHeight="1">
       <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
@@ -3438,8 +4806,11 @@
       <c r="AL24" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM24" s="25">
+        <v>33.103168099999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:39" ht="13.5" customHeight="1">
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
@@ -3554,8 +4925,11 @@
       <c r="AL25" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM25" s="25">
+        <v>123.20763460000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:39" ht="13.5" customHeight="1">
       <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
@@ -3670,8 +5044,11 @@
       <c r="AL26" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM26" s="25">
+        <v>104.4363992</v>
+      </c>
+    </row>
+    <row r="27" spans="2:39" ht="13.5" customHeight="1">
       <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
@@ -3786,8 +5163,11 @@
       <c r="AL27" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM27" s="25">
+        <v>87.668676509999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:39" ht="13.5" customHeight="1">
       <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
@@ -3902,8 +5282,11 @@
       <c r="AL28" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM28" s="25">
+        <v>74.492149889999993</v>
+      </c>
+    </row>
+    <row r="29" spans="2:39" ht="13.5" customHeight="1">
       <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
@@ -4017,8 +5400,11 @@
       <c r="AL29" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM29" s="25">
+        <v>62.788944829999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:39" ht="13.5" customHeight="1">
       <c r="B30" s="1" t="s">
         <v>73</v>
       </c>
@@ -4133,8 +5519,11 @@
       <c r="AL30" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM30" s="25">
+        <v>101.8299902</v>
+      </c>
+    </row>
+    <row r="31" spans="2:39" ht="13.5" customHeight="1">
       <c r="B31" s="1" t="s">
         <v>75</v>
       </c>
@@ -4249,8 +5638,11 @@
       <c r="AL31" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM31" s="25">
+        <v>72.671487290000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:39" ht="13.5" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
@@ -4364,8 +5756,11 @@
       <c r="AL32" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM32" s="25">
+        <v>49.567661430000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:39" ht="13.5" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>78</v>
       </c>
@@ -4479,8 +5874,11 @@
       <c r="AL33" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM33" s="25">
+        <v>35.637561460000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:39" ht="13.5" customHeight="1">
       <c r="B34" s="1" t="s">
         <v>79</v>
       </c>
@@ -4594,8 +5992,11 @@
       <c r="AL34" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM34" s="25">
+        <v>26.385149640000002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:39" ht="13.5" customHeight="1">
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
@@ -4710,8 +6111,11 @@
       <c r="AL35" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM35" s="25">
+        <v>127.4196888</v>
+      </c>
+    </row>
+    <row r="36" spans="2:39" ht="13.5" customHeight="1">
       <c r="B36" s="1" t="s">
         <v>82</v>
       </c>
@@ -4826,8 +6230,11 @@
       <c r="AL36" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM36" s="25">
+        <v>100.70642650000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:39" ht="13.5" customHeight="1">
       <c r="B37" s="1" t="s">
         <v>84</v>
       </c>
@@ -4941,8 +6348,11 @@
       <c r="AL37" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM37" s="25">
+        <v>76.093822939999995</v>
+      </c>
+    </row>
+    <row r="38" spans="2:39" ht="13.5" customHeight="1">
       <c r="B38" s="1" t="s">
         <v>86</v>
       </c>
@@ -5056,8 +6466,11 @@
       <c r="AL38" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM38" s="25">
+        <v>58.800198649999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:39" ht="13.5" customHeight="1">
       <c r="B39" s="1" t="s">
         <v>88</v>
       </c>
@@ -5171,8 +6584,11 @@
       <c r="AL39" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM39" s="25">
+        <v>46.26029896</v>
+      </c>
+    </row>
+    <row r="40" spans="2:39" ht="13.5" customHeight="1">
       <c r="B40" s="1" t="s">
         <v>89</v>
       </c>
@@ -5286,8 +6702,11 @@
       <c r="AL40" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM40" s="25">
+        <v>37.021449529999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:39" ht="13.5" customHeight="1">
       <c r="B41" s="1" t="s">
         <v>91</v>
       </c>
@@ -5402,8 +6821,11 @@
       <c r="AL41" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM41" s="25">
+        <v>156.45561960000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:39" ht="13.5" customHeight="1">
       <c r="B42" s="1" t="s">
         <v>93</v>
       </c>
@@ -5517,8 +6939,11 @@
       <c r="AL42" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM42" s="25">
+        <v>128.6319518</v>
+      </c>
+    </row>
+    <row r="43" spans="2:39" ht="13.5" customHeight="1">
       <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
@@ -5632,8 +7057,11 @@
       <c r="AL43" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM43" s="25">
+        <v>112.0877352</v>
+      </c>
+    </row>
+    <row r="44" spans="2:39" ht="13.5" customHeight="1">
       <c r="B44" s="1" t="s">
         <v>97</v>
       </c>
@@ -5747,8 +7175,11 @@
       <c r="AL44" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM44" s="25">
+        <v>98.269185429999993</v>
+      </c>
+    </row>
+    <row r="45" spans="2:39" ht="13.5" customHeight="1">
       <c r="B45" s="1" t="s">
         <v>98</v>
       </c>
@@ -5862,8 +7293,11 @@
       <c r="AL45" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM45" s="25">
+        <v>83.350726760000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:39" ht="13.5" customHeight="1">
       <c r="B46" s="1" t="s">
         <v>100</v>
       </c>
@@ -5977,8 +7411,11 @@
       <c r="AL46" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM46" s="25">
+        <v>70.855342019999995</v>
+      </c>
+    </row>
+    <row r="47" spans="2:39" ht="13.5" customHeight="1">
       <c r="B47" s="1" t="s">
         <v>101</v>
       </c>
@@ -6093,8 +7530,11 @@
       <c r="AL47" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="2:38" ht="13.5" customHeight="1">
+      <c r="AM47" s="25">
+        <v>190.59318060000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:39" ht="13.5" customHeight="1">
       <c r="B48" s="1" t="s">
         <v>103</v>
       </c>
@@ -6207,6 +7647,9 @@
       </c>
       <c r="AL48" s="20">
         <v>2</v>
+      </c>
+      <c r="AM48" s="25">
+        <v>169.4175434</v>
       </c>
     </row>
     <row r="49" spans="17:17" ht="13.5" customHeight="1">
@@ -9081,10 +10524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ1000"/>
+  <dimension ref="A1:AK1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AJ4" sqref="AJ4:AJ35"/>
+      <selection activeCell="AK2" activeCellId="2" sqref="B2:B35 L2:L35 AK2:AK35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -9114,7 +10557,7 @@
     <col min="36" max="36" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.5" customHeight="1">
+    <row r="1" spans="1:37" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -9144,7 +10587,7 @@
       <c r="AI1" s="14"/>
       <c r="AJ1" s="14"/>
     </row>
-    <row r="2" spans="1:36" s="12" customFormat="1" ht="13.5" customHeight="1">
+    <row r="2" spans="1:37" s="12" customFormat="1" ht="13.5" customHeight="1">
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -9250,12 +10693,15 @@
       <c r="AJ2" s="13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK2" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" ht="13.5" customHeight="1">
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1">
+    <row r="4" spans="1:37" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="18" t="s">
         <v>54</v>
@@ -9365,8 +10811,11 @@
       <c r="AJ4" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK4">
+        <v>60.189288419999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="18" t="s">
         <v>58</v>
@@ -9475,8 +10924,11 @@
       <c r="AJ5" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK5">
+        <v>40.683359469999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="19" t="s">
         <v>60</v>
@@ -9585,8 +11037,11 @@
       <c r="AJ6" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK6">
+        <v>21.451544340000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="19" t="s">
         <v>61</v>
@@ -9695,8 +11150,11 @@
       <c r="AJ7" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK7">
+        <v>5.7465885019999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="18" t="s">
         <v>63</v>
@@ -9806,8 +11264,11 @@
       <c r="AJ8" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK8">
+        <v>63.726450360000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="13.5" customHeight="1">
       <c r="B9" s="18" t="s">
         <v>64</v>
       </c>
@@ -9916,8 +11377,11 @@
       <c r="AJ9" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK9">
+        <v>64.271905689999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="13.5" customHeight="1">
       <c r="B10" s="18" t="s">
         <v>66</v>
       </c>
@@ -10026,8 +11490,11 @@
       <c r="AJ10" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK10">
+        <v>47.261879450000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" ht="13.5" customHeight="1">
       <c r="B11" s="18" t="s">
         <v>69</v>
       </c>
@@ -10135,8 +11602,11 @@
       <c r="AJ11" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK11">
+        <v>29.100196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="13.5" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>71</v>
       </c>
@@ -10244,8 +11714,11 @@
       <c r="AJ12" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK12">
+        <v>17.06638985</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="13.5" customHeight="1">
       <c r="B13" s="19" t="s">
         <v>74</v>
       </c>
@@ -10353,8 +11826,11 @@
       <c r="AJ13" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK13">
+        <v>9.506853864</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="13.5" customHeight="1">
       <c r="B14" s="19" t="s">
         <v>76</v>
       </c>
@@ -10462,8 +11938,11 @@
       <c r="AJ14" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK14">
+        <v>111.6510688</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="13.5" customHeight="1">
       <c r="B15" s="18" t="s">
         <v>80</v>
       </c>
@@ -10572,8 +12051,11 @@
       <c r="AJ15" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK15">
+        <v>75.656222549999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" ht="13.5" customHeight="1">
       <c r="B16" s="18" t="s">
         <v>83</v>
       </c>
@@ -10682,8 +12164,11 @@
       <c r="AJ16" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK16">
+        <v>50.12831731</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" ht="13.5" customHeight="1">
       <c r="B17" s="18" t="s">
         <v>85</v>
       </c>
@@ -10792,8 +12277,11 @@
       <c r="AJ17" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK17">
+        <v>61.798242469999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" ht="13.5" customHeight="1">
       <c r="B18" s="18" t="s">
         <v>87</v>
       </c>
@@ -10902,8 +12390,11 @@
       <c r="AJ18" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK18">
+        <v>47.716710669999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" ht="13.5" customHeight="1">
       <c r="B19" s="18" t="s">
         <v>90</v>
       </c>
@@ -11012,8 +12503,11 @@
       <c r="AJ19" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK19">
+        <v>32.104950270000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" ht="13.5" customHeight="1">
       <c r="B20" s="19" t="s">
         <v>92</v>
       </c>
@@ -11121,8 +12615,11 @@
       <c r="AJ20" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK20">
+        <v>20.934723680000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" ht="13.5" customHeight="1">
       <c r="B21" s="19" t="s">
         <v>94</v>
       </c>
@@ -11230,8 +12727,11 @@
       <c r="AJ21" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK21">
+        <v>13.129220180000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" ht="13.5" customHeight="1">
       <c r="B22" s="18" t="s">
         <v>96</v>
       </c>
@@ -11340,8 +12840,11 @@
       <c r="AJ22" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK22">
+        <v>102.3333861</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" ht="13.5" customHeight="1">
       <c r="B23" s="18" t="s">
         <v>99</v>
       </c>
@@ -11450,8 +12953,11 @@
       <c r="AJ23" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK23">
+        <v>75.062641900000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" ht="13.5" customHeight="1">
       <c r="B24" s="19" t="s">
         <v>102</v>
       </c>
@@ -11559,8 +13065,11 @@
       <c r="AJ24" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK24">
+        <v>52.498241399999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" ht="13.5" customHeight="1">
       <c r="B25" s="19" t="s">
         <v>104</v>
       </c>
@@ -11668,8 +13177,11 @@
       <c r="AJ25" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK25">
+        <v>37.057562740000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" ht="13.5" customHeight="1">
       <c r="B26" s="19" t="s">
         <v>105</v>
       </c>
@@ -11777,8 +13289,11 @@
       <c r="AJ26" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK26">
+        <v>26.286566969999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" ht="13.5" customHeight="1">
       <c r="B27" s="19" t="s">
         <v>106</v>
       </c>
@@ -11886,8 +13401,11 @@
       <c r="AJ27" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK27">
+        <v>18.933683519999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" ht="13.5" customHeight="1">
       <c r="B28" s="18" t="s">
         <v>107</v>
       </c>
@@ -11996,8 +13514,11 @@
       <c r="AJ28" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK28">
+        <v>142.8229451</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" ht="13.5" customHeight="1">
       <c r="B29" s="18" t="s">
         <v>108</v>
       </c>
@@ -12106,8 +13627,11 @@
       <c r="AJ29" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK29">
+        <v>121.0271814</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" ht="13.5" customHeight="1">
       <c r="B30" s="18" t="s">
         <v>109</v>
       </c>
@@ -12215,8 +13739,11 @@
       <c r="AJ30" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK30">
+        <v>98.456720970000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" ht="13.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
@@ -12328,8 +13855,11 @@
       <c r="AJ31" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" ht="13.5" customHeight="1">
+      <c r="AK31">
+        <v>95.937235340000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" ht="13.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
@@ -12441,8 +13971,11 @@
       <c r="AJ32" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:36" ht="13.5" customHeight="1">
+      <c r="AK32">
+        <v>71.570806910000002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:37" ht="13.5" customHeight="1">
       <c r="B33" s="16" t="s">
         <v>114</v>
       </c>
@@ -12551,8 +14084,11 @@
       <c r="AJ33" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:36" ht="13.5" customHeight="1">
+      <c r="AK33">
+        <v>86.620880700000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:37" ht="13.5" customHeight="1">
       <c r="B34" s="17" t="s">
         <v>115</v>
       </c>
@@ -12660,8 +14196,11 @@
       <c r="AJ34" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:36" ht="13.5" customHeight="1">
+      <c r="AK34">
+        <v>60.752835279999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:37" ht="13.5" customHeight="1">
       <c r="B35" s="17" t="s">
         <v>116</v>
       </c>
@@ -12769,92 +14308,95 @@
       <c r="AJ35" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:36" ht="13.5" customHeight="1">
+      <c r="AK35">
+        <v>43.422011179999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:37" ht="13.5" customHeight="1">
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="AH36" s="10"/>
       <c r="AI36" s="10"/>
       <c r="AJ36" s="10"/>
     </row>
-    <row r="37" spans="2:36" ht="13.5" customHeight="1">
+    <row r="37" spans="2:37" ht="13.5" customHeight="1">
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="AH37" s="11"/>
       <c r="AI37" s="11"/>
       <c r="AJ37" s="11"/>
     </row>
-    <row r="38" spans="2:36" ht="13.5" customHeight="1">
+    <row r="38" spans="2:37" ht="13.5" customHeight="1">
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="AH38" s="11"/>
       <c r="AI38" s="11"/>
       <c r="AJ38" s="11"/>
     </row>
-    <row r="39" spans="2:36" ht="13.5" customHeight="1">
+    <row r="39" spans="2:37" ht="13.5" customHeight="1">
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="AH39" s="11"/>
       <c r="AI39" s="11"/>
       <c r="AJ39" s="11"/>
     </row>
-    <row r="40" spans="2:36" ht="13.5" customHeight="1">
+    <row r="40" spans="2:37" ht="13.5" customHeight="1">
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="AH40" s="11"/>
       <c r="AI40" s="11"/>
       <c r="AJ40" s="11"/>
     </row>
-    <row r="41" spans="2:36" ht="13.5" customHeight="1">
+    <row r="41" spans="2:37" ht="13.5" customHeight="1">
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="AH41" s="10"/>
       <c r="AI41" s="10"/>
       <c r="AJ41" s="10"/>
     </row>
-    <row r="42" spans="2:36" ht="13.5" customHeight="1">
+    <row r="42" spans="2:37" ht="13.5" customHeight="1">
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="AH42" s="10"/>
       <c r="AI42" s="10"/>
       <c r="AJ42" s="10"/>
     </row>
-    <row r="43" spans="2:36" ht="13.5" customHeight="1">
+    <row r="43" spans="2:37" ht="13.5" customHeight="1">
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="AH43" s="11"/>
       <c r="AI43" s="11"/>
       <c r="AJ43" s="11"/>
     </row>
-    <row r="44" spans="2:36" ht="13.5" customHeight="1">
+    <row r="44" spans="2:37" ht="13.5" customHeight="1">
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="AH44" s="11"/>
       <c r="AI44" s="11"/>
       <c r="AJ44" s="11"/>
     </row>
-    <row r="45" spans="2:36" ht="13.5" customHeight="1">
+    <row r="45" spans="2:37" ht="13.5" customHeight="1">
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="AH45" s="11"/>
       <c r="AI45" s="11"/>
       <c r="AJ45" s="11"/>
     </row>
-    <row r="46" spans="2:36" ht="13.5" customHeight="1">
+    <row r="46" spans="2:37" ht="13.5" customHeight="1">
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="AH46" s="11"/>
       <c r="AI46" s="11"/>
       <c r="AJ46" s="11"/>
     </row>
-    <row r="47" spans="2:36" ht="13.5" customHeight="1">
+    <row r="47" spans="2:37" ht="13.5" customHeight="1">
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="AH47" s="10"/>
       <c r="AI47" s="10"/>
       <c r="AJ47" s="10"/>
     </row>
-    <row r="48" spans="2:36" ht="13.5" customHeight="1">
+    <row r="48" spans="2:37" ht="13.5" customHeight="1">
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="AH48" s="10"/>

</xml_diff>

<commit_message>
Tweak to chemkin parameters; input files now stable for both burke and burke_mod. Results for both in spreadsheet
</commit_message>
<xml_diff>
--- a/src/Burke_input_files/Burke_data.xlsx
+++ b/src/Burke_input_files/Burke_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1500" windowWidth="34760" windowHeight="19720" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="940" yWindow="860" windowWidth="34760" windowHeight="19720" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
   <si>
     <t>Burke C&amp;F 2010 data</t>
   </si>
@@ -390,6 +390,9 @@
   <si>
     <t>sim</t>
   </si>
+  <si>
+    <t>sim_mod</t>
+  </si>
 </sst>
 </file>
 
@@ -467,8 +470,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -506,11 +511,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1145,6 +1152,309 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AN$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sim_mod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$3:$B$48</c:f>
+              <c:strCache>
+                <c:ptCount val="46"/>
+                <c:pt idx="1">
+                  <c:v>Burkef1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Burkef2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Burkef3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Burkef4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Burkef5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Burkef6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Burkef7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Burkef8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Burkef9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Burkef10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Burkef11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Burkef12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Burkef13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Burkef14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Burkef15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Burkef16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Burkef17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Burkef18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Burkef19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Burkef20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Burkef21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Burkef22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Burkef23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Burkef24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Burkef25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Burkef26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Burkef27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Burkef28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Burkef29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Burkef30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Burkef31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Burkef32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Burkef33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Burkef34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Burkef35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Burkef36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Burkef37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Burkef38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Burkef39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Burkef40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Burkef41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Burkef42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Burkef43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Burkef44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Burkef45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AN$3:$AN$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="1">
+                  <c:v>94.14821818</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.95420269</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.11028004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.60652506</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.39854114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.07531612</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69.49900332</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.88667105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.5909689</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.56884426</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.65235178</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44.73934812</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.42600107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.60775471</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.59707203</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>103.5555097</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82.88056121</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>65.55216734</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50.33282712</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39.74905295</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32.23384594</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>121.8398854</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>102.6818894</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>85.45880442</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>72.01544724999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60.42479348</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100.8846507</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>72.39777081</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49.8948729</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36.09525102</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.90444011</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>126.6803986</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100.5247942</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>76.33782171</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>59.31676522</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>47.4412661</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.35861824</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>155.618115</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>130.9003438</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>109.4421484</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>98.28986832</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>83.15770062</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>70.26464057</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>189.3813735</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>169.5222165</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1164,6 +1474,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1674,6 +1985,231 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$AL$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sim_mod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$3:$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="1">
+                  <c:v>Burkef46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Burkef47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Burkef48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Burkef49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Burkef50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Burkef51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Burkef52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Burkef53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Burkef54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Burkef55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Burkef56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Burkef57</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Burkef58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Burkef59</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Burkef60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Burkef61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Burkef62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Burkef63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Burkef64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Burkef65</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Burkef66</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Burkef67</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Burkef68</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Burkef69</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Burkef70</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Burkef71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Burkef72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Burkef73</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Burkef74</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Burkef75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Burkef76</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Burkef77</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$AL$3:$AL$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="1">
+                  <c:v>59.26400024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.6827946</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.57161858</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.70965924</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.41650198</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63.26445078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.31954902</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.09093057</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.37578825</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.291337105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>108.2443903</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73.35224734000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48.21404384</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.73717421</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46.88075134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.2779701</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20.27704589</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.69757437</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100.8946819</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>73.16912962</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50.38499918</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>35.16522197</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.78988607</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17.95616228</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>140.8768137</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>118.1077879</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>94.83903635999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>94.14821818</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>69.95420269</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>85.56884426</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60.03500029</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43.03331805</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1736,7 +2272,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1747,7 +2283,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -2130,13 +2666,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN1000"/>
+  <dimension ref="A1:AO1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AM2" activeCellId="2" sqref="B2:B48 N2:N48 AM2:AM48"/>
+      <selection pane="bottomRight" activeCell="AN49" sqref="AN49:AN80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -2163,11 +2699,11 @@
     <col min="36" max="36" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.83203125" customWidth="1"/>
-    <col min="40" max="40" width="7.6640625" customWidth="1"/>
+    <col min="39" max="40" width="9.83203125" customWidth="1"/>
+    <col min="41" max="41" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="13.5" customHeight="1">
+    <row r="1" spans="1:41" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2196,8 +2732,9 @@
       <c r="AK1" s="14"/>
       <c r="AL1" s="14"/>
       <c r="AM1" s="24"/>
-    </row>
-    <row r="2" spans="1:40" s="12" customFormat="1" ht="13.5" customHeight="1">
+      <c r="AN1" s="24"/>
+    </row>
+    <row r="2" spans="1:41" s="12" customFormat="1" ht="13.5" customHeight="1">
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -2312,11 +2849,14 @@
       <c r="AM2" s="13" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN2" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" ht="13.5" customHeight="1">
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:40" ht="13.5" customHeight="1">
+    <row r="4" spans="1:41" ht="13.5" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
@@ -2434,11 +2974,14 @@
       <c r="AM4" s="25">
         <v>95.937235340000001</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AN4" s="25">
+        <v>94.148218180000001</v>
+      </c>
+      <c r="AO4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="13.5" customHeight="1">
+    <row r="5" spans="1:41" ht="13.5" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -2556,11 +3099,14 @@
       <c r="AM5" s="25">
         <v>71.570806910000002</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AN5" s="25">
+        <v>69.954202690000002</v>
+      </c>
+      <c r="AO5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="13.5" customHeight="1">
+    <row r="6" spans="1:41" ht="13.5" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
@@ -2678,8 +3224,11 @@
       <c r="AM6" s="25">
         <v>52.903966689999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN6" s="25">
+        <v>51.110280039999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="13.5" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
@@ -2796,8 +3345,11 @@
       <c r="AM7" s="25">
         <v>36.523679520000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN7" s="25">
+        <v>35.606525060000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="13.5" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>41</v>
       </c>
@@ -2915,8 +3467,11 @@
       <c r="AM8" s="25">
         <v>26.55322194</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN8" s="25">
+        <v>25.398541139999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" ht="13.5" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>42</v>
       </c>
@@ -3032,8 +3587,11 @@
       <c r="AM9" s="25">
         <v>19.968800989999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN9" s="25">
+        <v>19.07531612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" ht="13.5" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
@@ -3150,8 +3708,11 @@
       <c r="AM10" s="25">
         <v>70.417389639999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN10" s="25">
+        <v>69.49900332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" ht="13.5" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
@@ -3268,8 +3829,11 @@
       <c r="AM11" s="25">
         <v>45.014318760000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN11" s="25">
+        <v>44.886671049999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" ht="13.5" customHeight="1">
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
@@ -3386,8 +3950,11 @@
       <c r="AM12" s="25">
         <v>28.064514689999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN12" s="25">
+        <v>28.5909689</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" ht="13.5" customHeight="1">
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
@@ -3505,8 +4072,11 @@
       <c r="AM13" s="25">
         <v>86.620880700000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN13" s="25">
+        <v>85.568844260000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" ht="13.5" customHeight="1">
       <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
@@ -3623,11 +4193,14 @@
       <c r="AM14" s="25">
         <v>61.730400439999997</v>
       </c>
-      <c r="AN14" s="1" t="s">
+      <c r="AN14" s="25">
+        <v>61.652351779999996</v>
+      </c>
+      <c r="AO14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="13.5" customHeight="1">
+    <row r="15" spans="1:41" ht="13.5" customHeight="1">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -3744,8 +4317,11 @@
       <c r="AM15" s="25">
         <v>45.24507887</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" ht="13.5" customHeight="1">
+      <c r="AN15" s="25">
+        <v>44.739348120000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" ht="13.5" customHeight="1">
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
@@ -3862,8 +4438,11 @@
       <c r="AM16" s="25">
         <v>32.684779290000002</v>
       </c>
-    </row>
-    <row r="17" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN16" s="25">
+        <v>32.426001069999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:40" ht="13.5" customHeight="1">
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -3980,8 +4559,11 @@
       <c r="AM17" s="25">
         <v>23.89041847</v>
       </c>
-    </row>
-    <row r="18" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN17" s="25">
+        <v>23.607754709999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:40" ht="13.5" customHeight="1">
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
@@ -4098,8 +4680,11 @@
       <c r="AM18" s="25">
         <v>17.85782549</v>
       </c>
-    </row>
-    <row r="19" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN18" s="25">
+        <v>17.59707203</v>
+      </c>
+    </row>
+    <row r="19" spans="2:40" ht="13.5" customHeight="1">
       <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
@@ -4217,8 +4802,11 @@
       <c r="AM19" s="25">
         <v>104.7389546</v>
       </c>
-    </row>
-    <row r="20" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN19" s="25">
+        <v>103.5555097</v>
+      </c>
+    </row>
+    <row r="20" spans="2:40" ht="13.5" customHeight="1">
       <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
@@ -4336,8 +4924,11 @@
       <c r="AM20" s="25">
         <v>84.367675500000004</v>
       </c>
-    </row>
-    <row r="21" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN20" s="25">
+        <v>82.880561209999996</v>
+      </c>
+    </row>
+    <row r="21" spans="2:40" ht="13.5" customHeight="1">
       <c r="B21" s="1" t="s">
         <v>56</v>
       </c>
@@ -4455,8 +5046,11 @@
       <c r="AM21" s="25">
         <v>67.175088669999994</v>
       </c>
-    </row>
-    <row r="22" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN21" s="25">
+        <v>65.552167339999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:40" ht="13.5" customHeight="1">
       <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
@@ -4573,8 +5167,11 @@
       <c r="AM22" s="25">
         <v>50.649937549999997</v>
       </c>
-    </row>
-    <row r="23" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN22" s="25">
+        <v>50.332827119999997</v>
+      </c>
+    </row>
+    <row r="23" spans="2:40" ht="13.5" customHeight="1">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
@@ -4691,8 +5288,11 @@
       <c r="AM23" s="25">
         <v>41.147652229999998</v>
       </c>
-    </row>
-    <row r="24" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN23" s="25">
+        <v>39.749052949999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:40" ht="13.5" customHeight="1">
       <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
@@ -4809,8 +5409,11 @@
       <c r="AM24" s="25">
         <v>33.103168099999998</v>
       </c>
-    </row>
-    <row r="25" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN24" s="25">
+        <v>32.233845940000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:40" ht="13.5" customHeight="1">
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
@@ -4928,8 +5531,11 @@
       <c r="AM25" s="25">
         <v>123.20763460000001</v>
       </c>
-    </row>
-    <row r="26" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN25" s="25">
+        <v>121.8398854</v>
+      </c>
+    </row>
+    <row r="26" spans="2:40" ht="13.5" customHeight="1">
       <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
@@ -5047,8 +5653,11 @@
       <c r="AM26" s="25">
         <v>104.4363992</v>
       </c>
-    </row>
-    <row r="27" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN26" s="25">
+        <v>102.6818894</v>
+      </c>
+    </row>
+    <row r="27" spans="2:40" ht="13.5" customHeight="1">
       <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
@@ -5166,8 +5775,11 @@
       <c r="AM27" s="25">
         <v>87.668676509999997</v>
       </c>
-    </row>
-    <row r="28" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN27" s="25">
+        <v>85.458804420000007</v>
+      </c>
+    </row>
+    <row r="28" spans="2:40" ht="13.5" customHeight="1">
       <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
@@ -5285,8 +5897,11 @@
       <c r="AM28" s="25">
         <v>74.492149889999993</v>
       </c>
-    </row>
-    <row r="29" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN28" s="25">
+        <v>72.015447249999994</v>
+      </c>
+    </row>
+    <row r="29" spans="2:40" ht="13.5" customHeight="1">
       <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
@@ -5403,8 +6018,11 @@
       <c r="AM29" s="25">
         <v>62.788944829999998</v>
       </c>
-    </row>
-    <row r="30" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN29" s="25">
+        <v>60.424793479999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:40" ht="13.5" customHeight="1">
       <c r="B30" s="1" t="s">
         <v>73</v>
       </c>
@@ -5522,8 +6140,11 @@
       <c r="AM30" s="25">
         <v>101.8299902</v>
       </c>
-    </row>
-    <row r="31" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN30" s="25">
+        <v>100.88465069999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:40" ht="13.5" customHeight="1">
       <c r="B31" s="1" t="s">
         <v>75</v>
       </c>
@@ -5641,8 +6262,11 @@
       <c r="AM31" s="25">
         <v>72.671487290000002</v>
       </c>
-    </row>
-    <row r="32" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN31" s="25">
+        <v>72.397770809999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:40" ht="13.5" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
@@ -5759,8 +6383,11 @@
       <c r="AM32" s="25">
         <v>49.567661430000001</v>
       </c>
-    </row>
-    <row r="33" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN32" s="25">
+        <v>49.894872900000003</v>
+      </c>
+    </row>
+    <row r="33" spans="2:40" ht="13.5" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>78</v>
       </c>
@@ -5877,8 +6504,11 @@
       <c r="AM33" s="25">
         <v>35.637561460000001</v>
       </c>
-    </row>
-    <row r="34" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN33" s="25">
+        <v>36.095251019999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:40" ht="13.5" customHeight="1">
       <c r="B34" s="1" t="s">
         <v>79</v>
       </c>
@@ -5995,8 +6625,11 @@
       <c r="AM34" s="25">
         <v>26.385149640000002</v>
       </c>
-    </row>
-    <row r="35" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN34" s="25">
+        <v>26.904440109999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:40" ht="13.5" customHeight="1">
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
@@ -6114,8 +6747,11 @@
       <c r="AM35" s="25">
         <v>127.4196888</v>
       </c>
-    </row>
-    <row r="36" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN35" s="25">
+        <v>126.6803986</v>
+      </c>
+    </row>
+    <row r="36" spans="2:40" ht="13.5" customHeight="1">
       <c r="B36" s="1" t="s">
         <v>82</v>
       </c>
@@ -6233,8 +6869,11 @@
       <c r="AM36" s="25">
         <v>100.70642650000001</v>
       </c>
-    </row>
-    <row r="37" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN36" s="25">
+        <v>100.5247942</v>
+      </c>
+    </row>
+    <row r="37" spans="2:40" ht="13.5" customHeight="1">
       <c r="B37" s="1" t="s">
         <v>84</v>
       </c>
@@ -6351,8 +6990,11 @@
       <c r="AM37" s="25">
         <v>76.093822939999995</v>
       </c>
-    </row>
-    <row r="38" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN37" s="25">
+        <v>76.33782171</v>
+      </c>
+    </row>
+    <row r="38" spans="2:40" ht="13.5" customHeight="1">
       <c r="B38" s="1" t="s">
         <v>86</v>
       </c>
@@ -6469,8 +7111,11 @@
       <c r="AM38" s="25">
         <v>58.800198649999999</v>
       </c>
-    </row>
-    <row r="39" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN38" s="25">
+        <v>59.316765220000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:40" ht="13.5" customHeight="1">
       <c r="B39" s="1" t="s">
         <v>88</v>
       </c>
@@ -6587,8 +7232,11 @@
       <c r="AM39" s="25">
         <v>46.26029896</v>
       </c>
-    </row>
-    <row r="40" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN39" s="25">
+        <v>47.4412661</v>
+      </c>
+    </row>
+    <row r="40" spans="2:40" ht="13.5" customHeight="1">
       <c r="B40" s="1" t="s">
         <v>89</v>
       </c>
@@ -6705,8 +7353,11 @@
       <c r="AM40" s="25">
         <v>37.021449529999998</v>
       </c>
-    </row>
-    <row r="41" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN40" s="25">
+        <v>38.358618239999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:40" ht="13.5" customHeight="1">
       <c r="B41" s="1" t="s">
         <v>91</v>
       </c>
@@ -6824,8 +7475,11 @@
       <c r="AM41" s="25">
         <v>156.45561960000001</v>
       </c>
-    </row>
-    <row r="42" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN41" s="25">
+        <v>155.61811499999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:40" ht="13.5" customHeight="1">
       <c r="B42" s="1" t="s">
         <v>93</v>
       </c>
@@ -6942,8 +7596,11 @@
       <c r="AM42" s="25">
         <v>128.6319518</v>
       </c>
-    </row>
-    <row r="43" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN42" s="25">
+        <v>130.9003438</v>
+      </c>
+    </row>
+    <row r="43" spans="2:40" ht="13.5" customHeight="1">
       <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
@@ -7060,8 +7717,11 @@
       <c r="AM43" s="25">
         <v>112.0877352</v>
       </c>
-    </row>
-    <row r="44" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN43" s="25">
+        <v>109.44214839999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:40" ht="13.5" customHeight="1">
       <c r="B44" s="1" t="s">
         <v>97</v>
       </c>
@@ -7178,8 +7838,11 @@
       <c r="AM44" s="25">
         <v>98.269185429999993</v>
       </c>
-    </row>
-    <row r="45" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN44" s="25">
+        <v>98.289868319999997</v>
+      </c>
+    </row>
+    <row r="45" spans="2:40" ht="13.5" customHeight="1">
       <c r="B45" s="1" t="s">
         <v>98</v>
       </c>
@@ -7282,7 +7945,7 @@
         <v>5</v>
       </c>
       <c r="AI45" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AJ45" s="6">
         <v>0.5</v>
@@ -7296,8 +7959,11 @@
       <c r="AM45" s="25">
         <v>83.350726760000001</v>
       </c>
-    </row>
-    <row r="46" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN45" s="25">
+        <v>83.15770062</v>
+      </c>
+    </row>
+    <row r="46" spans="2:40" ht="13.5" customHeight="1">
       <c r="B46" s="1" t="s">
         <v>100</v>
       </c>
@@ -7400,7 +8066,7 @@
         <v>5</v>
       </c>
       <c r="AI46" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AJ46" s="6">
         <v>0.5</v>
@@ -7414,8 +8080,11 @@
       <c r="AM46" s="25">
         <v>70.855342019999995</v>
       </c>
-    </row>
-    <row r="47" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN46" s="25">
+        <v>70.264640569999997</v>
+      </c>
+    </row>
+    <row r="47" spans="2:40" ht="13.5" customHeight="1">
       <c r="B47" s="1" t="s">
         <v>101</v>
       </c>
@@ -7533,8 +8202,11 @@
       <c r="AM47" s="25">
         <v>190.59318060000001</v>
       </c>
-    </row>
-    <row r="48" spans="2:39" ht="13.5" customHeight="1">
+      <c r="AN47" s="25">
+        <v>189.3813735</v>
+      </c>
+    </row>
+    <row r="48" spans="2:40" ht="13.5" customHeight="1">
       <c r="B48" s="1" t="s">
         <v>103</v>
       </c>
@@ -7650,6 +8322,9 @@
       </c>
       <c r="AM48" s="25">
         <v>169.4175434</v>
+      </c>
+      <c r="AN48" s="25">
+        <v>169.52221650000001</v>
       </c>
     </row>
     <row r="49" spans="17:17" ht="13.5" customHeight="1">
@@ -10524,10 +11199,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK1000"/>
+  <dimension ref="A1:AL1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AK2" activeCellId="2" sqref="B2:B35 L2:L35 AK2:AK35"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AL4" sqref="AL4:AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -10557,7 +11232,7 @@
     <col min="36" max="36" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="13.5" customHeight="1">
+    <row r="1" spans="1:38" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -10587,7 +11262,7 @@
       <c r="AI1" s="14"/>
       <c r="AJ1" s="14"/>
     </row>
-    <row r="2" spans="1:37" s="12" customFormat="1" ht="13.5" customHeight="1">
+    <row r="2" spans="1:38" s="12" customFormat="1" ht="13.5" customHeight="1">
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -10696,12 +11371,15 @@
       <c r="AK2" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL2" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="13.5" customHeight="1">
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:37" ht="13.5" customHeight="1">
+    <row r="4" spans="1:38" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="18" t="s">
         <v>54</v>
@@ -10814,8 +11492,11 @@
       <c r="AK4">
         <v>60.189288419999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL4">
+        <v>59.264000240000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="18" t="s">
         <v>58</v>
@@ -10927,8 +11608,11 @@
       <c r="AK5">
         <v>40.683359469999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL5">
+        <v>39.682794600000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="19" t="s">
         <v>60</v>
@@ -11040,8 +11724,11 @@
       <c r="AK6">
         <v>21.451544340000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL6">
+        <v>20.571618579999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="19" t="s">
         <v>61</v>
@@ -11153,8 +11840,11 @@
       <c r="AK7">
         <v>5.7465885019999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL7">
+        <v>5.7096592399999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="18" t="s">
         <v>63</v>
@@ -11267,8 +11957,11 @@
       <c r="AK8">
         <v>63.726450360000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL8">
+        <v>61.41650198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="13.5" customHeight="1">
       <c r="B9" s="18" t="s">
         <v>64</v>
       </c>
@@ -11380,8 +12073,11 @@
       <c r="AK9">
         <v>64.271905689999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL9">
+        <v>63.264450779999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="13.5" customHeight="1">
       <c r="B10" s="18" t="s">
         <v>66</v>
       </c>
@@ -11493,8 +12189,11 @@
       <c r="AK10">
         <v>47.261879450000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL10">
+        <v>46.319549019999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="13.5" customHeight="1">
       <c r="B11" s="18" t="s">
         <v>69</v>
       </c>
@@ -11605,8 +12304,11 @@
       <c r="AK11">
         <v>29.100196</v>
       </c>
-    </row>
-    <row r="12" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL11">
+        <v>28.090930570000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="13.5" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>71</v>
       </c>
@@ -11717,8 +12419,11 @@
       <c r="AK12">
         <v>17.06638985</v>
       </c>
-    </row>
-    <row r="13" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL12">
+        <v>16.375788249999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="13.5" customHeight="1">
       <c r="B13" s="19" t="s">
         <v>74</v>
       </c>
@@ -11829,8 +12534,11 @@
       <c r="AK13">
         <v>9.506853864</v>
       </c>
-    </row>
-    <row r="14" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL13">
+        <v>9.2913371050000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="13.5" customHeight="1">
       <c r="B14" s="19" t="s">
         <v>76</v>
       </c>
@@ -11941,8 +12649,11 @@
       <c r="AK14">
         <v>111.6510688</v>
       </c>
-    </row>
-    <row r="15" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL14">
+        <v>108.24439030000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" ht="13.5" customHeight="1">
       <c r="B15" s="18" t="s">
         <v>80</v>
       </c>
@@ -12054,8 +12765,11 @@
       <c r="AK15">
         <v>75.656222549999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL15">
+        <v>73.352247340000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="13.5" customHeight="1">
       <c r="B16" s="18" t="s">
         <v>83</v>
       </c>
@@ -12167,8 +12881,11 @@
       <c r="AK16">
         <v>50.12831731</v>
       </c>
-    </row>
-    <row r="17" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL16">
+        <v>48.214043840000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" ht="13.5" customHeight="1">
       <c r="B17" s="18" t="s">
         <v>85</v>
       </c>
@@ -12280,8 +12997,11 @@
       <c r="AK17">
         <v>61.798242469999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL17">
+        <v>60.737174209999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" ht="13.5" customHeight="1">
       <c r="B18" s="18" t="s">
         <v>87</v>
       </c>
@@ -12393,8 +13113,11 @@
       <c r="AK18">
         <v>47.716710669999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL18">
+        <v>46.880751340000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" ht="13.5" customHeight="1">
       <c r="B19" s="18" t="s">
         <v>90</v>
       </c>
@@ -12506,8 +13229,11 @@
       <c r="AK19">
         <v>32.104950270000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL19">
+        <v>31.277970100000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" ht="13.5" customHeight="1">
       <c r="B20" s="19" t="s">
         <v>92</v>
       </c>
@@ -12618,8 +13344,11 @@
       <c r="AK20">
         <v>20.934723680000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL20">
+        <v>20.27704589</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" ht="13.5" customHeight="1">
       <c r="B21" s="19" t="s">
         <v>94</v>
       </c>
@@ -12716,7 +13445,7 @@
         <v>5</v>
       </c>
       <c r="AG21" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH21" s="6">
         <v>0.5</v>
@@ -12730,8 +13459,11 @@
       <c r="AK21">
         <v>13.129220180000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL21">
+        <v>12.69757437</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" ht="13.5" customHeight="1">
       <c r="B22" s="18" t="s">
         <v>96</v>
       </c>
@@ -12843,8 +13575,11 @@
       <c r="AK22">
         <v>102.3333861</v>
       </c>
-    </row>
-    <row r="23" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL22">
+        <v>100.89468189999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" ht="13.5" customHeight="1">
       <c r="B23" s="18" t="s">
         <v>99</v>
       </c>
@@ -12956,8 +13691,11 @@
       <c r="AK23">
         <v>75.062641900000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL23">
+        <v>73.169129620000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" ht="13.5" customHeight="1">
       <c r="B24" s="19" t="s">
         <v>102</v>
       </c>
@@ -13068,8 +13806,11 @@
       <c r="AK24">
         <v>52.498241399999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL24">
+        <v>50.384999180000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" ht="13.5" customHeight="1">
       <c r="B25" s="19" t="s">
         <v>104</v>
       </c>
@@ -13180,8 +13921,11 @@
       <c r="AK25">
         <v>37.057562740000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL25">
+        <v>35.165221969999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" ht="13.5" customHeight="1">
       <c r="B26" s="19" t="s">
         <v>105</v>
       </c>
@@ -13292,8 +14036,11 @@
       <c r="AK26">
         <v>26.286566969999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL26">
+        <v>24.789886070000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" ht="13.5" customHeight="1">
       <c r="B27" s="19" t="s">
         <v>106</v>
       </c>
@@ -13404,8 +14151,11 @@
       <c r="AK27">
         <v>18.933683519999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL27">
+        <v>17.956162280000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" ht="13.5" customHeight="1">
       <c r="B28" s="18" t="s">
         <v>107</v>
       </c>
@@ -13517,8 +14267,11 @@
       <c r="AK28">
         <v>142.8229451</v>
       </c>
-    </row>
-    <row r="29" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL28">
+        <v>140.87681370000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" ht="13.5" customHeight="1">
       <c r="B29" s="18" t="s">
         <v>108</v>
       </c>
@@ -13630,8 +14383,11 @@
       <c r="AK29">
         <v>121.0271814</v>
       </c>
-    </row>
-    <row r="30" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL29">
+        <v>118.10778790000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" ht="13.5" customHeight="1">
       <c r="B30" s="18" t="s">
         <v>109</v>
       </c>
@@ -13742,8 +14498,11 @@
       <c r="AK30">
         <v>98.456720970000006</v>
       </c>
-    </row>
-    <row r="31" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL30">
+        <v>94.839036359999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" ht="13.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
@@ -13858,8 +14617,11 @@
       <c r="AK31">
         <v>95.937235340000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:37" ht="13.5" customHeight="1">
+      <c r="AL31">
+        <v>94.148218180000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" ht="13.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
@@ -13974,8 +14736,11 @@
       <c r="AK32">
         <v>71.570806910000002</v>
       </c>
-    </row>
-    <row r="33" spans="2:37" ht="13.5" customHeight="1">
+      <c r="AL32">
+        <v>69.954202690000002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:38" ht="13.5" customHeight="1">
       <c r="B33" s="16" t="s">
         <v>114</v>
       </c>
@@ -14087,8 +14852,11 @@
       <c r="AK33">
         <v>86.620880700000001</v>
       </c>
-    </row>
-    <row r="34" spans="2:37" ht="13.5" customHeight="1">
+      <c r="AL33">
+        <v>85.568844260000006</v>
+      </c>
+    </row>
+    <row r="34" spans="2:38" ht="13.5" customHeight="1">
       <c r="B34" s="17" t="s">
         <v>115</v>
       </c>
@@ -14199,8 +14967,11 @@
       <c r="AK34">
         <v>60.752835279999999</v>
       </c>
-    </row>
-    <row r="35" spans="2:37" ht="13.5" customHeight="1">
+      <c r="AL34">
+        <v>60.035000289999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:38" ht="13.5" customHeight="1">
       <c r="B35" s="17" t="s">
         <v>116</v>
       </c>
@@ -14311,92 +15082,95 @@
       <c r="AK35">
         <v>43.422011179999998</v>
       </c>
-    </row>
-    <row r="36" spans="2:37" ht="13.5" customHeight="1">
+      <c r="AL35">
+        <v>43.033318049999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:38" ht="13.5" customHeight="1">
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="AH36" s="10"/>
       <c r="AI36" s="10"/>
       <c r="AJ36" s="10"/>
     </row>
-    <row r="37" spans="2:37" ht="13.5" customHeight="1">
+    <row r="37" spans="2:38" ht="13.5" customHeight="1">
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="AH37" s="11"/>
       <c r="AI37" s="11"/>
       <c r="AJ37" s="11"/>
     </row>
-    <row r="38" spans="2:37" ht="13.5" customHeight="1">
+    <row r="38" spans="2:38" ht="13.5" customHeight="1">
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="AH38" s="11"/>
       <c r="AI38" s="11"/>
       <c r="AJ38" s="11"/>
     </row>
-    <row r="39" spans="2:37" ht="13.5" customHeight="1">
+    <row r="39" spans="2:38" ht="13.5" customHeight="1">
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="AH39" s="11"/>
       <c r="AI39" s="11"/>
       <c r="AJ39" s="11"/>
     </row>
-    <row r="40" spans="2:37" ht="13.5" customHeight="1">
+    <row r="40" spans="2:38" ht="13.5" customHeight="1">
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="AH40" s="11"/>
       <c r="AI40" s="11"/>
       <c r="AJ40" s="11"/>
     </row>
-    <row r="41" spans="2:37" ht="13.5" customHeight="1">
+    <row r="41" spans="2:38" ht="13.5" customHeight="1">
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="AH41" s="10"/>
       <c r="AI41" s="10"/>
       <c r="AJ41" s="10"/>
     </row>
-    <row r="42" spans="2:37" ht="13.5" customHeight="1">
+    <row r="42" spans="2:38" ht="13.5" customHeight="1">
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="AH42" s="10"/>
       <c r="AI42" s="10"/>
       <c r="AJ42" s="10"/>
     </row>
-    <row r="43" spans="2:37" ht="13.5" customHeight="1">
+    <row r="43" spans="2:38" ht="13.5" customHeight="1">
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="AH43" s="11"/>
       <c r="AI43" s="11"/>
       <c r="AJ43" s="11"/>
     </row>
-    <row r="44" spans="2:37" ht="13.5" customHeight="1">
+    <row r="44" spans="2:38" ht="13.5" customHeight="1">
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="AH44" s="11"/>
       <c r="AI44" s="11"/>
       <c r="AJ44" s="11"/>
     </row>
-    <row r="45" spans="2:37" ht="13.5" customHeight="1">
+    <row r="45" spans="2:38" ht="13.5" customHeight="1">
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="AH45" s="11"/>
       <c r="AI45" s="11"/>
       <c r="AJ45" s="11"/>
     </row>
-    <row r="46" spans="2:37" ht="13.5" customHeight="1">
+    <row r="46" spans="2:38" ht="13.5" customHeight="1">
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="AH46" s="11"/>
       <c r="AI46" s="11"/>
       <c r="AJ46" s="11"/>
     </row>
-    <row r="47" spans="2:37" ht="13.5" customHeight="1">
+    <row r="47" spans="2:38" ht="13.5" customHeight="1">
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="AH47" s="10"/>
       <c r="AI47" s="10"/>
       <c r="AJ47" s="10"/>
     </row>
-    <row r="48" spans="2:37" ht="13.5" customHeight="1">
+    <row r="48" spans="2:38" ht="13.5" customHeight="1">
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="AH48" s="10"/>

</xml_diff>

<commit_message>
Add a few more pressure steps in B14 and B36
</commit_message>
<xml_diff>
--- a/src/Burke_input_files/Burke_data.xlsx
+++ b/src/Burke_input_files/Burke_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
@@ -1468,11 +1468,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2135247176"/>
-        <c:axId val="2135240264"/>
+        <c:axId val="-2136236664"/>
+        <c:axId val="-2136234760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135247176"/>
+        <c:axId val="-2136236664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135240264"/>
+        <c:crossAx val="-2136234760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1490,7 +1490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135240264"/>
+        <c:axId val="-2136234760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1501,14 +1501,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135247176"/>
+        <c:crossAx val="-2136236664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2223,11 +2222,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105585928"/>
-        <c:axId val="2105601944"/>
+        <c:axId val="-2129273272"/>
+        <c:axId val="-2129270296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105585928"/>
+        <c:axId val="-2129273272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,7 +2235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105601944"/>
+        <c:crossAx val="-2129270296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2244,7 +2243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105601944"/>
+        <c:axId val="-2129270296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105585928"/>
+        <c:crossAx val="-2129273272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2672,10 +2671,10 @@
   <dimension ref="A1:AO1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J16" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="S14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AI40" sqref="AI40"/>
+      <selection pane="bottomRight" activeCell="AH40" sqref="AH40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4545,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="AH17" s="22">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="AI17" s="6">
         <v>0.1</v>
@@ -7218,7 +7217,7 @@
         <v>5</v>
       </c>
       <c r="AH39" s="22">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="AI39" s="6">
         <v>0.5</v>

</xml_diff>